<commit_message>
Updated Jul 31 2018
</commit_message>
<xml_diff>
--- a/meta-analysis - variable names output.xlsx
+++ b/meta-analysis - variable names output.xlsx
@@ -492,7 +492,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -500,8 +500,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF222222"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -511,6 +516,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -544,6 +555,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13:H15"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,7 +849,7 @@
     <col min="8" max="8" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>149</v>
       </c>
@@ -848,7 +861,7 @@
       </c>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>148</v>
       </c>
@@ -871,7 +884,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>151</v>
       </c>
@@ -888,7 +901,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -907,8 +920,12 @@
       <c r="H4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="6" t="str">
+        <f>IF(ISNUMBER(MATCH(H4,G$4:G$84,0)),"matches old variable", "new")</f>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -927,8 +944,12 @@
       <c r="H5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="6" t="str">
+        <f t="shared" ref="I5:I68" si="0">IF(ISNUMBER(MATCH(H5,G$4:G$84,0)),"matches old variable", "new")</f>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -947,8 +968,12 @@
       <c r="H6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -967,8 +992,12 @@
       <c r="H7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -987,8 +1016,12 @@
       <c r="H8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -1007,8 +1040,12 @@
       <c r="H9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -1027,8 +1064,12 @@
       <c r="H10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -1047,8 +1088,12 @@
       <c r="H11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -1067,8 +1112,12 @@
       <c r="H12" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>9</v>
       </c>
@@ -1084,11 +1133,15 @@
       <c r="G13" t="s">
         <v>69</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="5" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1107,8 +1160,12 @@
       <c r="H14" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>11</v>
       </c>
@@ -1127,8 +1184,12 @@
       <c r="H15" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -1147,8 +1208,12 @@
       <c r="H16" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>13</v>
       </c>
@@ -1167,8 +1232,12 @@
       <c r="H17" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>14</v>
       </c>
@@ -1187,8 +1256,12 @@
       <c r="H18" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>15</v>
       </c>
@@ -1207,8 +1280,12 @@
       <c r="H19" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>16</v>
       </c>
@@ -1227,8 +1304,12 @@
       <c r="H20" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>17</v>
       </c>
@@ -1247,8 +1328,12 @@
       <c r="H21" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>18</v>
       </c>
@@ -1267,8 +1352,12 @@
       <c r="H22" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>19</v>
       </c>
@@ -1287,8 +1376,12 @@
       <c r="H23" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>20</v>
       </c>
@@ -1307,8 +1400,12 @@
       <c r="H24" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>21</v>
       </c>
@@ -1327,8 +1424,12 @@
       <c r="H25" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>22</v>
       </c>
@@ -1347,8 +1448,12 @@
       <c r="H26" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>23</v>
       </c>
@@ -1367,8 +1472,12 @@
       <c r="H27" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>24</v>
       </c>
@@ -1387,8 +1496,12 @@
       <c r="H28" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>25</v>
       </c>
@@ -1407,8 +1520,12 @@
       <c r="H29" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>26</v>
       </c>
@@ -1427,8 +1544,12 @@
       <c r="H30" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>27</v>
       </c>
@@ -1447,8 +1568,12 @@
       <c r="H31" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>28</v>
       </c>
@@ -1467,8 +1592,12 @@
       <c r="H32" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I32" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>29</v>
       </c>
@@ -1487,8 +1616,12 @@
       <c r="H33" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I33" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>30</v>
       </c>
@@ -1507,8 +1640,12 @@
       <c r="H34" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I34" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>31</v>
       </c>
@@ -1527,8 +1664,12 @@
       <c r="H35" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I35" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>32</v>
       </c>
@@ -1547,8 +1688,12 @@
       <c r="H36" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I36" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>33</v>
       </c>
@@ -1567,8 +1712,12 @@
       <c r="H37" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I37" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>34</v>
       </c>
@@ -1587,8 +1736,12 @@
       <c r="H38" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I38" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>35</v>
       </c>
@@ -1607,8 +1760,12 @@
       <c r="H39" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I39" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>36</v>
       </c>
@@ -1627,8 +1784,12 @@
       <c r="H40" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I40" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>37</v>
       </c>
@@ -1647,8 +1808,12 @@
       <c r="H41" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I41" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>38</v>
       </c>
@@ -1667,8 +1832,12 @@
       <c r="H42" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I42" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>39</v>
       </c>
@@ -1687,8 +1856,12 @@
       <c r="H43" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I43" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>40</v>
       </c>
@@ -1707,8 +1880,12 @@
       <c r="H44" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I44" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>41</v>
       </c>
@@ -1727,8 +1904,12 @@
       <c r="H45" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I45" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>42</v>
       </c>
@@ -1747,8 +1928,12 @@
       <c r="H46" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I46" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>43</v>
       </c>
@@ -1767,8 +1952,12 @@
       <c r="H47" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I47" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>44</v>
       </c>
@@ -1787,8 +1976,12 @@
       <c r="H48" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I48" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>45</v>
       </c>
@@ -1807,8 +2000,12 @@
       <c r="H49" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I49" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>46</v>
       </c>
@@ -1827,8 +2024,12 @@
       <c r="H50" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I50" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>47</v>
       </c>
@@ -1847,8 +2048,12 @@
       <c r="H51" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I51" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>48</v>
       </c>
@@ -1867,8 +2072,12 @@
       <c r="H52" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I52" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>49</v>
       </c>
@@ -1887,8 +2096,12 @@
       <c r="H53" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I53" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>50</v>
       </c>
@@ -1907,8 +2120,12 @@
       <c r="H54" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I54" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>51</v>
       </c>
@@ -1927,8 +2144,12 @@
       <c r="H55" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I55" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>52</v>
       </c>
@@ -1947,8 +2168,12 @@
       <c r="H56" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I56" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>53</v>
       </c>
@@ -1967,8 +2192,12 @@
       <c r="H57" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I57" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
         <v>50</v>
       </c>
@@ -1978,8 +2207,12 @@
       <c r="H58" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I58" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
         <v>51</v>
       </c>
@@ -1989,8 +2222,12 @@
       <c r="H59" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I59" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>52</v>
       </c>
@@ -2000,8 +2237,12 @@
       <c r="H60" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I60" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
         <v>61</v>
       </c>
@@ -2011,8 +2252,12 @@
       <c r="H61" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I61" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
         <v>62</v>
       </c>
@@ -2022,8 +2267,12 @@
       <c r="H62" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I62" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
         <v>53</v>
       </c>
@@ -2033,162 +2282,258 @@
       <c r="H63" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I63" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G64" t="s">
         <v>120</v>
       </c>
       <c r="H64" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="65" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I64" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="65" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G65" t="s">
         <v>121</v>
       </c>
       <c r="H65" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="66" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I65" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="66" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G66" t="s">
         <v>122</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H66" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="67" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I66" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="67" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G67" t="s">
         <v>123</v>
       </c>
       <c r="H67" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="68" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I67" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="68" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G68" t="s">
         <v>124</v>
       </c>
       <c r="H68" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="69" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I68" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="69" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G69" t="s">
         <v>125</v>
       </c>
       <c r="H69" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="70" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I69" s="6" t="str">
+        <f t="shared" ref="I69:I83" si="1">IF(ISNUMBER(MATCH(H69,G$4:G$84,0)),"matches old variable", "new")</f>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="70" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G70" t="s">
         <v>126</v>
       </c>
       <c r="H70" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="71" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I70" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="71" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G71" t="s">
         <v>127</v>
       </c>
       <c r="H71" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="72" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I71" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="72" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G72" t="s">
         <v>128</v>
       </c>
       <c r="H72" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="73" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I72" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="73" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G73" t="s">
         <v>129</v>
       </c>
       <c r="H73" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="74" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I73" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="74" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G74" t="s">
         <v>130</v>
       </c>
       <c r="H74" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="75" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I74" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="75" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G75" t="s">
         <v>131</v>
       </c>
       <c r="H75" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="76" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I75" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="76" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G76" t="s">
         <v>132</v>
       </c>
       <c r="H76" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="77" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I76" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="77" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G77" t="s">
         <v>133</v>
       </c>
       <c r="H77" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="78" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I77" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="78" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G78" t="s">
         <v>134</v>
       </c>
       <c r="H78" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="79" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I78" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="79" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G79" t="s">
         <v>135</v>
       </c>
       <c r="H79" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="80" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I79" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="80" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G80" t="s">
         <v>136</v>
       </c>
       <c r="H80" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="81" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I80" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="81" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G81" t="s">
         <v>137</v>
       </c>
       <c r="H81" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="82" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I81" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="82" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="G82" t="s">
         <v>138</v>
       </c>
       <c r="H82" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="83" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I82" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="83" spans="7:9" ht="21" x14ac:dyDescent="0.25">
       <c r="H83" t="s">
         <v>134</v>
+      </c>
+      <c r="I83" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>matches old variable</v>
+      </c>
+    </row>
+    <row r="84" spans="7:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="I84" s="6">
+        <f t="shared" ref="I69:I85" si="2">IF(ISNUMBER(MATCH(H84,G$4:G$60,0)),1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="7:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="I85" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>